<commit_message>
adding beam bending cases
</commit_message>
<xml_diff>
--- a/fusion_tube/psd.xlsx
+++ b/fusion_tube/psd.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaina/projects/mylammps/fusion_tube/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB5DBC6-5BCC-5C46-9F6E-2C15C929CB46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F0C430-8017-D445-89E7-E1DF743C6B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="3520" windowWidth="19100" windowHeight="17440" xr2:uid="{A1589F0B-647C-9E4A-BA53-9F1372460473}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{A1589F0B-647C-9E4A-BA53-9F1372460473}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -110,9 +111,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="189" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,16 +127,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -143,15 +156,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2589,7 +2620,7 @@
   <dimension ref="B1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2653,7 +2684,7 @@
         <v>0.78539816339744828</v>
       </c>
       <c r="E3">
-        <f>(C3/$C$3)^$E$1</f>
+        <f t="shared" ref="E3:E13" si="0">(C3/$C$3)^$E$1</f>
         <v>1</v>
       </c>
       <c r="F3">
@@ -2661,7 +2692,7 @@
         <v>0.57342048119840738</v>
       </c>
       <c r="G3">
-        <f>(F3/D3)/(F$3/D$3)</f>
+        <f t="shared" ref="G3:G13" si="1">(F3/D3)/(F$3/D$3)</f>
         <v>1</v>
       </c>
       <c r="H3" s="1">
@@ -2675,19 +2706,19 @@
         <v>1</v>
       </c>
       <c r="O3">
-        <f>N3*D3</f>
+        <f t="shared" ref="O3:O13" si="2">N3*D3</f>
         <v>0.78539816339744828</v>
       </c>
       <c r="P3">
-        <f>O3/SUM(O$3:O$13)</f>
+        <f t="shared" ref="P3:P13" si="3">O3/SUM(O$3:O$13)</f>
         <v>3.6294874074934397E-2</v>
       </c>
       <c r="Q3">
-        <f>N3/SUM(N$3:N$13)</f>
+        <f t="shared" ref="Q3:Q13" si="4">N3/SUM(N$3:N$13)</f>
         <v>1.1290122272024207E-5</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R11" si="0">P3+R4</f>
+        <f t="shared" ref="R3:R11" si="5">P3+R4</f>
         <v>1</v>
       </c>
     </row>
@@ -2699,23 +2730,23 @@
         <v>0.1</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D13" si="1">C4^2*PI()/4</f>
+        <f t="shared" ref="D4:D13" si="6">C4^2*PI()/4</f>
         <v>7.8539816339744835E-3</v>
       </c>
       <c r="E4">
-        <f>(C4/$C$3)^$E$1</f>
+        <f t="shared" si="0"/>
         <v>0.42657951880159267</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F12" si="2">E4-E5</f>
+        <f t="shared" ref="F4:F12" si="7">E4-E5</f>
         <v>1.6309549884757191E-2</v>
       </c>
       <c r="G4">
-        <f>(F4/D4)/(F$3/D$3)</f>
+        <f t="shared" si="1"/>
         <v>2.8442566004394205</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:H13" si="3">G4/$G$14</f>
+        <f t="shared" ref="H4:H13" si="8">G4/$G$14</f>
         <v>7.9847492257268966E-4</v>
       </c>
       <c r="I4" s="1">
@@ -2726,19 +2757,19 @@
         <v>3</v>
       </c>
       <c r="O4">
-        <f>N4*D4</f>
+        <f t="shared" si="2"/>
         <v>2.356194490192345E-2</v>
       </c>
       <c r="P4">
-        <f>O4/SUM(O$3:O$13)</f>
+        <f t="shared" si="3"/>
         <v>1.0888462222480319E-3</v>
       </c>
       <c r="Q4">
-        <f>N4/SUM(N$3:N$13)</f>
+        <f t="shared" si="4"/>
         <v>3.387036681607262E-5</v>
       </c>
       <c r="R4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.96370512592506563</v>
       </c>
     </row>
@@ -2750,46 +2781,46 @@
         <v>0.09</v>
       </c>
       <c r="D5">
+        <f t="shared" si="6"/>
+        <v>6.3617251235193305E-3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.41026996891683548</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="7"/>
+        <v>1.7495459196186613E-2</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="1"/>
-        <v>6.3617251235193305E-3</v>
-      </c>
-      <c r="E5">
-        <f>(C5/$C$3)^$E$1</f>
-        <v>0.41026996891683548</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="2"/>
-        <v>1.7495459196186613E-2</v>
-      </c>
-      <c r="G5">
-        <f>(F5/D5)/(F$3/D$3)</f>
         <v>3.7667528540016719</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.0574494906629654E-3</v>
       </c>
       <c r="I5" s="1">
         <v>1.06E-3</v>
       </c>
       <c r="N5">
-        <f t="shared" ref="N5:N13" si="4">N4*3</f>
+        <f t="shared" ref="N5:N13" si="9">N4*3</f>
         <v>9</v>
       </c>
       <c r="O5">
-        <f>N5*D5</f>
+        <f t="shared" si="2"/>
         <v>5.7255526111673977E-2</v>
       </c>
       <c r="P5">
-        <f>O5/SUM(O$3:O$13)</f>
+        <f t="shared" si="3"/>
         <v>2.6458963200627172E-3</v>
       </c>
       <c r="Q5">
-        <f>N5/SUM(N$3:N$13)</f>
+        <f t="shared" si="4"/>
         <v>1.0161110044821786E-4</v>
       </c>
       <c r="R5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.9626162797028176</v>
       </c>
     </row>
@@ -2801,46 +2832,46 @@
         <v>0.08</v>
       </c>
       <c r="D6">
+        <f t="shared" si="6"/>
+        <v>5.0265482457436689E-3</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.39277450972064887</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="7"/>
+        <v>1.893407347721271E-2</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="1"/>
-        <v>5.0265482457436689E-3</v>
-      </c>
-      <c r="E6">
-        <f>(C6/$C$3)^$E$1</f>
-        <v>0.39277450972064887</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="2"/>
-        <v>1.893407347721271E-2</v>
-      </c>
-      <c r="G6">
-        <f>(F6/D6)/(F$3/D$3)</f>
         <v>5.1593012070854902</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.4483829030124504E-3</v>
       </c>
       <c r="I6" s="1">
         <v>1.4499999999999999E-3</v>
       </c>
       <c r="N6">
+        <f t="shared" si="9"/>
+        <v>27</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="2"/>
+        <v>0.13571680263507907</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="3"/>
+        <v>6.271754240148664E-3</v>
+      </c>
+      <c r="Q6">
         <f t="shared" si="4"/>
-        <v>27</v>
-      </c>
-      <c r="O6">
-        <f>N6*D6</f>
-        <v>0.13571680263507907</v>
-      </c>
-      <c r="P6">
-        <f>O6/SUM(O$3:O$13)</f>
-        <v>6.271754240148664E-3</v>
-      </c>
-      <c r="Q6">
-        <f>N6/SUM(N$3:N$13)</f>
         <v>3.0483330134465356E-4</v>
       </c>
       <c r="R6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.95997038338275487</v>
       </c>
     </row>
@@ -2852,46 +2883,46 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D7">
+        <f t="shared" si="6"/>
+        <v>3.8484510006474969E-3</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.37384043624343616</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="7"/>
+        <v>2.0725601901908308E-2</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="1"/>
-        <v>3.8484510006474969E-3</v>
-      </c>
-      <c r="E7">
-        <f>(C7/$C$3)^$E$1</f>
-        <v>0.37384043624343616</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="2"/>
-        <v>2.0725601901908308E-2</v>
-      </c>
-      <c r="G7">
-        <f>(F7/D7)/(F$3/D$3)</f>
         <v>7.3762881036600572</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2.0707629092023131E-3</v>
       </c>
       <c r="I7" s="1">
         <v>2.0699999999999998E-3</v>
       </c>
       <c r="N7">
+        <f t="shared" si="9"/>
+        <v>81</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="2"/>
+        <v>0.31172453105244724</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="3"/>
+        <v>1.4405435520341462E-2</v>
+      </c>
+      <c r="Q7">
         <f t="shared" si="4"/>
-        <v>81</v>
-      </c>
-      <c r="O7">
-        <f>N7*D7</f>
-        <v>0.31172453105244724</v>
-      </c>
-      <c r="P7">
-        <f>O7/SUM(O$3:O$13)</f>
-        <v>1.4405435520341462E-2</v>
-      </c>
-      <c r="Q7">
-        <f>N7/SUM(N$3:N$13)</f>
         <v>9.1449990403396069E-4</v>
       </c>
       <c r="R7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.95369862914260617</v>
       </c>
     </row>
@@ -2903,46 +2934,46 @@
         <v>0.06</v>
       </c>
       <c r="D8">
+        <f t="shared" si="6"/>
+        <v>2.8274333882308137E-3</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.35311483434152785</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="7"/>
+        <v>2.303506921177656E-2</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="1"/>
-        <v>2.8274333882308137E-3</v>
-      </c>
-      <c r="E8">
-        <f>(C8/$C$3)^$E$1</f>
-        <v>0.35311483434152785</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="2"/>
-        <v>2.303506921177656E-2</v>
-      </c>
-      <c r="G8">
-        <f>(F8/D8)/(F$3/D$3)</f>
         <v>11.158705603315605</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.1326099731094348E-3</v>
       </c>
       <c r="I8" s="1">
         <v>3.13E-3</v>
       </c>
       <c r="N8">
+        <f t="shared" si="9"/>
+        <v>243</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="2"/>
+        <v>0.68706631334008772</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="3"/>
+        <v>3.1750755840752612E-2</v>
+      </c>
+      <c r="Q8">
         <f t="shared" si="4"/>
-        <v>243</v>
-      </c>
-      <c r="O8">
-        <f>N8*D8</f>
-        <v>0.68706631334008772</v>
-      </c>
-      <c r="P8">
-        <f>O8/SUM(O$3:O$13)</f>
-        <v>3.1750755840752612E-2</v>
-      </c>
-      <c r="Q8">
-        <f>N8/SUM(N$3:N$13)</f>
         <v>2.7434997121018822E-3</v>
       </c>
       <c r="R8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.93929319362226471</v>
       </c>
     </row>
@@ -2954,46 +2985,46 @@
         <v>0.05</v>
       </c>
       <c r="D9">
+        <f t="shared" si="6"/>
+        <v>1.9634954084936209E-3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.33007976512975129</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="7"/>
+        <v>2.6157724330025611E-2</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="1"/>
-        <v>1.9634954084936209E-3</v>
-      </c>
-      <c r="E9">
-        <f>(C9/$C$3)^$E$1</f>
-        <v>0.33007976512975129</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="2"/>
-        <v>2.6157724330025611E-2</v>
-      </c>
-      <c r="G9">
-        <f>(F9/D9)/(F$3/D$3)</f>
         <v>18.246801561993639</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>5.1224680157764902E-3</v>
       </c>
       <c r="I9" s="1">
         <v>5.1200000000000004E-3</v>
       </c>
       <c r="N9">
+        <f t="shared" si="9"/>
+        <v>729</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="2"/>
+        <v>1.4313881527918497</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="3"/>
+        <v>6.6147408001567945E-2</v>
+      </c>
+      <c r="Q9">
         <f t="shared" si="4"/>
-        <v>729</v>
-      </c>
-      <c r="O9">
-        <f>N9*D9</f>
-        <v>1.4313881527918497</v>
-      </c>
-      <c r="P9">
-        <f>O9/SUM(O$3:O$13)</f>
-        <v>6.6147408001567945E-2</v>
-      </c>
-      <c r="Q9">
-        <f>N9/SUM(N$3:N$13)</f>
         <v>8.2304991363056461E-3</v>
       </c>
       <c r="R9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.90754243778151211</v>
       </c>
     </row>
@@ -3005,46 +3036,46 @@
         <v>0.04</v>
       </c>
       <c r="D10">
+        <f t="shared" si="6"/>
+        <v>1.2566370614359172E-3</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.30392204079972568</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="7"/>
+        <v>3.0687962635991384E-2</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="1"/>
-        <v>1.2566370614359172E-3</v>
-      </c>
-      <c r="E10">
-        <f>(C10/$C$3)^$E$1</f>
-        <v>0.30392204079972568</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="2"/>
-        <v>3.0687962635991384E-2</v>
-      </c>
-      <c r="G10">
-        <f>(F10/D10)/(F$3/D$3)</f>
         <v>33.448363419823878</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>9.3900386440874846E-3</v>
       </c>
       <c r="I10" s="1">
         <v>9.3900000000000008E-3</v>
       </c>
       <c r="N10">
+        <f t="shared" si="9"/>
+        <v>2187</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="2"/>
+        <v>2.7482652533603509</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="3"/>
+        <v>0.12700302336301045</v>
+      </c>
+      <c r="Q10">
         <f t="shared" si="4"/>
-        <v>2187</v>
-      </c>
-      <c r="O10">
-        <f>N10*D10</f>
-        <v>2.7482652533603509</v>
-      </c>
-      <c r="P10">
-        <f>O10/SUM(O$3:O$13)</f>
-        <v>0.12700302336301045</v>
-      </c>
-      <c r="Q10">
-        <f>N10/SUM(N$3:N$13)</f>
         <v>2.4691497408916938E-2</v>
       </c>
       <c r="R10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.84139502977994418</v>
       </c>
     </row>
@@ -3056,46 +3087,46 @@
         <v>0.03</v>
       </c>
       <c r="D11">
+        <f t="shared" si="6"/>
+        <v>7.0685834705770342E-4</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.2732340781637343</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="7"/>
+        <v>3.8064522609925572E-2</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="1"/>
-        <v>7.0685834705770342E-4</v>
-      </c>
-      <c r="E11">
-        <f>(C11/$C$3)^$E$1</f>
-        <v>0.2732340781637343</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="2"/>
-        <v>3.8064522609925572E-2</v>
-      </c>
-      <c r="G11">
-        <f>(F11/D11)/(F$3/D$3)</f>
         <v>73.757243415228544</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2.0706046429162184E-2</v>
       </c>
       <c r="I11" s="1">
         <v>2.0709999999999999E-2</v>
       </c>
       <c r="N11">
+        <f t="shared" si="9"/>
+        <v>6561</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="2"/>
+        <v>4.6376976150455924</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="3"/>
+        <v>0.21431760192508012</v>
+      </c>
+      <c r="Q11">
         <f t="shared" si="4"/>
-        <v>6561</v>
-      </c>
-      <c r="O11">
-        <f>N11*D11</f>
-        <v>4.6376976150455924</v>
-      </c>
-      <c r="P11">
-        <f>O11/SUM(O$3:O$13)</f>
-        <v>0.21431760192508012</v>
-      </c>
-      <c r="Q11">
-        <f>N11/SUM(N$3:N$13)</f>
         <v>7.4074492226750818E-2</v>
       </c>
       <c r="R11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.71439200641693368</v>
       </c>
     </row>
@@ -3107,42 +3138,42 @@
         <v>0.02</v>
       </c>
       <c r="D12">
+        <f t="shared" si="6"/>
+        <v>3.1415926535897931E-4</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.23516955555380872</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="7"/>
+        <v>5.3199469692810336E-2</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="1"/>
-        <v>3.1415926535897931E-4</v>
-      </c>
-      <c r="E12">
-        <f>(C12/$C$3)^$E$1</f>
-        <v>0.23516955555380872</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="2"/>
-        <v>5.3199469692810336E-2</v>
-      </c>
-      <c r="G12">
-        <f>(F12/D12)/(F$3/D$3)</f>
         <v>231.93917656039807</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>6.5112836871689186E-2</v>
       </c>
       <c r="I12" s="1">
         <v>6.5110000000000001E-2</v>
       </c>
       <c r="N12">
+        <f t="shared" si="9"/>
+        <v>19683</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="2"/>
+        <v>6.1835968200607896</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="3"/>
+        <v>0.28575680256677349</v>
+      </c>
+      <c r="Q12">
         <f t="shared" si="4"/>
-        <v>19683</v>
-      </c>
-      <c r="O12">
-        <f>N12*D12</f>
-        <v>6.1835968200607896</v>
-      </c>
-      <c r="P12">
-        <f>O12/SUM(O$3:O$13)</f>
-        <v>0.28575680256677349</v>
-      </c>
-      <c r="Q12">
-        <f>N12/SUM(N$3:N$13)</f>
         <v>0.22222347668025244</v>
       </c>
       <c r="R12">
@@ -3158,11 +3189,11 @@
         <v>0.01</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>7.8539816339744827E-5</v>
       </c>
       <c r="E13">
-        <f>(C13/$C$3)^$E$1</f>
+        <f t="shared" si="0"/>
         <v>0.18197008586099839</v>
       </c>
       <c r="F13">
@@ -3170,30 +3201,30 @@
         <v>0.18197008586099839</v>
       </c>
       <c r="G13">
-        <f>(F13/D13)/(F$3/D$3)</f>
+        <f t="shared" si="1"/>
         <v>3173.4144807784692</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.89088019746149805</v>
       </c>
       <c r="I13" s="1">
         <v>0.89088000000000001</v>
       </c>
       <c r="N13">
+        <f t="shared" si="9"/>
+        <v>59049</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="2"/>
+        <v>4.6376976150455924</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="3"/>
+        <v>0.21431760192508012</v>
+      </c>
+      <c r="Q13">
         <f t="shared" si="4"/>
-        <v>59049</v>
-      </c>
-      <c r="O13">
-        <f>N13*D13</f>
-        <v>4.6376976150455924</v>
-      </c>
-      <c r="P13">
-        <f>O13/SUM(O$3:O$13)</f>
-        <v>0.21431760192508012</v>
-      </c>
-      <c r="Q13">
-        <f>N13/SUM(N$3:N$13)</f>
         <v>0.66667043004075732</v>
       </c>
       <c r="R13">
@@ -3240,23 +3271,23 @@
       <c r="B18" t="s">
         <v>1</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>1</v>
       </c>
       <c r="D18">
         <f>C18^2*PI()/4</f>
         <v>0.78539816339744828</v>
       </c>
-      <c r="F18">
-        <v>0.8</v>
+      <c r="F18" s="2">
+        <v>0.7</v>
       </c>
       <c r="G18">
         <f>(F18/D18)/(F$3/D$3)</f>
-        <v>1.3951367735035514</v>
+        <v>1.2207446768156074</v>
       </c>
       <c r="H18" s="1">
         <f>G18/$G$23</f>
-        <v>2.0133636443210253E-2</v>
+        <v>1.1843980591568928E-2</v>
       </c>
       <c r="I18" s="1"/>
     </row>
@@ -3264,11 +3295,11 @@
       <c r="B19" t="s">
         <v>2</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>0.1</v>
       </c>
       <c r="D19">
-        <f t="shared" ref="D19:D22" si="5">C19^2*PI()/4</f>
+        <f t="shared" ref="D19:D22" si="10">C19^2*PI()/4</f>
         <v>7.8539816339744835E-3</v>
       </c>
       <c r="E19">
@@ -3277,15 +3308,15 @@
       </c>
       <c r="F19">
         <f>(E19-E20)*(1-F$18)</f>
-        <v>7.6466633609491002E-3</v>
+        <v>1.1469995041423655E-2</v>
       </c>
       <c r="G19">
         <f>(F19/D19)/(F$3/D$3)</f>
-        <v>1.3335176561827937</v>
+        <v>2.0002764842741914</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" ref="H19:H22" si="6">G19/$G$23</f>
-        <v>1.9244392514120676E-2</v>
+        <f t="shared" ref="H19:H22" si="11">G19/$G$23</f>
+        <v>1.9407199808001947E-2</v>
       </c>
       <c r="I19" s="1"/>
     </row>
@@ -3293,28 +3324,28 @@
       <c r="B20" t="s">
         <v>3</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>0.09</v>
       </c>
       <c r="D20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>6.3617251235193305E-3</v>
       </c>
       <c r="E20">
-        <f t="shared" ref="E20:E22" si="7">(C20/$C$19)^$E$1</f>
+        <f t="shared" ref="E20:E22" si="12">(C20/$C$19)^$E$1</f>
         <v>0.96176668319525449</v>
       </c>
       <c r="F20">
-        <f t="shared" ref="F20:F22" si="8">(E20-E21)*(1-F$18)</f>
-        <v>8.2026719169909102E-3</v>
+        <f t="shared" ref="F20:F22" si="13">(E20-E21)*(1-F$18)</f>
+        <v>1.2304007875486368E-2</v>
       </c>
       <c r="G20">
         <f>(F20/D20)/(F$3/D$3)</f>
-        <v>1.7660261161078534</v>
+        <v>2.6490391741617807</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="6"/>
-        <v>2.5486051580189122E-2</v>
+        <f t="shared" si="11"/>
+        <v>2.5701663223240179E-2</v>
       </c>
       <c r="I20" s="1"/>
     </row>
@@ -3322,28 +3353,28 @@
       <c r="B21" t="s">
         <v>4</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>0.08</v>
       </c>
       <c r="D21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>5.0265482457436689E-3</v>
       </c>
       <c r="E21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.92075332361029993</v>
       </c>
       <c r="F21">
-        <f t="shared" si="8"/>
-        <v>8.8771601273333473E-3</v>
+        <f t="shared" si="13"/>
+        <v>1.3315740191000028E-2</v>
       </c>
       <c r="G21">
         <f>(F21/D21)/(F$3/D$3)</f>
-        <v>2.4189165113129341</v>
+        <v>3.6283747669694031</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="6"/>
-        <v>3.4908108330447593E-2</v>
+        <f t="shared" si="11"/>
+        <v>3.5203430442986315E-2</v>
       </c>
       <c r="I21" s="1"/>
     </row>
@@ -3351,35 +3382,39 @@
       <c r="B22" t="s">
         <v>5</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>3.8484510006474969E-3</v>
       </c>
       <c r="E22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.87636752297363318</v>
       </c>
       <c r="F22">
-        <f t="shared" si="8"/>
-        <v>0.1752735045947266</v>
+        <f t="shared" si="13"/>
+        <v>0.26291025689209002</v>
       </c>
       <c r="G22">
         <f>(F22/D22)/(F$3/D$3)</f>
-        <v>62.380232571670085</v>
+        <v>93.570348857505167</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="6"/>
-        <v>0.90022781113203232</v>
+        <f t="shared" si="11"/>
+        <v>0.90784372593420259</v>
       </c>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="G23">
         <f>SUM(G18:G22)</f>
-        <v>69.293829628777218</v>
+        <v>103.06878395972615</v>
+      </c>
+      <c r="H23">
+        <f>SUM(H18:H22)</f>
+        <v>1</v>
       </c>
       <c r="I23" s="1"/>
     </row>

</xml_diff>

<commit_message>
3d case working for small length
</commit_message>
<xml_diff>
--- a/fusion_tube/psd.xlsx
+++ b/fusion_tube/psd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaina/projects/mylammps/fusion_tube/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F0C430-8017-D445-89E7-E1DF743C6B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D986D6F-5630-DB48-A8E9-9AC8237A65C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{A1589F0B-647C-9E4A-BA53-9F1372460473}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A1589F0B-647C-9E4A-BA53-9F1372460473}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Diameter</t>
   </si>
@@ -113,7 +112,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -130,6 +129,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -176,10 +181,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -2617,10 +2623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F78EA03-871C-B64F-95D3-3F1B251107D7}">
-  <dimension ref="B1:R23"/>
+  <dimension ref="B1:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3336,7 +3342,7 @@
         <v>0.96176668319525449</v>
       </c>
       <c r="F20">
-        <f t="shared" ref="F20:F22" si="13">(E20-E21)*(1-F$18)</f>
+        <f t="shared" ref="F20:F21" si="13">(E20-E21)*(1-F$18)</f>
         <v>1.2304007875486368E-2</v>
       </c>
       <c r="G20">
@@ -3394,7 +3400,7 @@
         <v>0.87636752297363318</v>
       </c>
       <c r="F22">
-        <f t="shared" si="13"/>
+        <f>(E22-E23)*(1-F$18)</f>
         <v>0.26291025689209002</v>
       </c>
       <c r="G22">
@@ -3417,6 +3423,123 @@
         <v>1</v>
       </c>
       <c r="I23" s="1"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <f>C29^2*PI()/4</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G29">
+        <f>(F29/D29)/(F$3/D$3)</f>
+        <v>1.2207446768156074</v>
+      </c>
+      <c r="H29" s="1">
+        <f>G29/$G$34</f>
+        <v>9.1869094933264964E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ref="D30:D31" si="14">C30^2*PI()/4</f>
+        <v>7.0685834705770348E-2</v>
+      </c>
+      <c r="E30">
+        <f>(C30/$C$30)^$E$1</f>
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <f>(E30-E31)*(1-F$29)</f>
+        <v>4.1793310921248564E-2</v>
+      </c>
+      <c r="G30">
+        <f>(F30/D30)/(F$3/D$3)</f>
+        <v>0.80982479100974247</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" ref="H30:H31" si="15">G30/$G$34</f>
+        <v>6.0944661088883231E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="14"/>
+        <v>3.1415926535897934E-2</v>
+      </c>
+      <c r="E31">
+        <f>(C31/$C$30)^$E$1</f>
+        <v>0.86068896359583813</v>
+      </c>
+      <c r="F31">
+        <f>(E31-E32)*(1-F$29)</f>
+        <v>0.25820668907875149</v>
+      </c>
+      <c r="G31">
+        <f>(F31/D31)/(F$3/D$3)</f>
+        <v>11.257301471823876</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="15"/>
+        <v>0.84718624397785181</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C32" s="2"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C33" s="2"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G34" s="3">
+        <f>SUM(G29:G33)</f>
+        <v>13.287870939649226</v>
+      </c>
+      <c r="H34" s="1">
+        <f>SUM(H29:H33)</f>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
3d case working wo scaling
</commit_message>
<xml_diff>
--- a/fusion_tube/psd.xlsx
+++ b/fusion_tube/psd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaina/projects/mylammps/fusion_tube/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D986D6F-5630-DB48-A8E9-9AC8237A65C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D324E2-4507-C341-AB14-78A3C2C51401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A1589F0B-647C-9E4A-BA53-9F1372460473}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="23">
   <si>
     <t>Diameter</t>
   </si>
@@ -2623,10 +2623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F78EA03-871C-B64F-95D3-3F1B251107D7}">
-  <dimension ref="B1:R34"/>
+  <dimension ref="B1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3527,17 +3527,241 @@
       <c r="C32" s="2"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C33" s="2"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G34" s="3">
         <f>SUM(G29:G33)</f>
         <v>13.287870939649226</v>
       </c>
       <c r="H34" s="1">
         <f>SUM(H29:H33)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" t="s">
+        <v>21</v>
+      </c>
+      <c r="G37" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <f>C38^2*PI()/4</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G38">
+        <f>(F38/D38)/(F$3/D$3)</f>
+        <v>1.2207446768156074</v>
+      </c>
+      <c r="H38" s="1">
+        <f>G38/$G$43</f>
+        <v>6.03726176284025E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="D39">
+        <f t="shared" ref="D39:D40" si="16">C39^2*PI()/4</f>
+        <v>0.13854423602330987</v>
+      </c>
+      <c r="E39">
+        <f>(C39/$C$30)^$E$1</f>
+        <v>1.1325760489937422</v>
+      </c>
+      <c r="F39">
+        <f>(E39-E40)*(1-F$38)</f>
+        <v>3.9772814698122667E-2</v>
+      </c>
+      <c r="G39">
+        <f>(F39/D39)/(F$3/D$3)</f>
+        <v>0.39320093800378036</v>
+      </c>
+      <c r="H39" s="1">
+        <f>G39/$G$43</f>
+        <v>1.9445974520368212E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="16"/>
+        <v>7.0685834705770348E-2</v>
+      </c>
+      <c r="E40">
+        <f>(C40/$C$30)^$E$1</f>
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <f>(E40-E41)*(1-F$39)</f>
+        <v>0.96022718530187734</v>
+      </c>
+      <c r="G40">
+        <f>(F40/D40)/(F$3/D$3)</f>
+        <v>18.606225793506361</v>
+      </c>
+      <c r="H40" s="1">
+        <f>G40/$G$43</f>
+        <v>0.92018140785122926</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C41" s="2"/>
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C42" s="2"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G43" s="3">
+        <f>SUM(G38:G42)</f>
+        <v>20.220171408325751</v>
+      </c>
+      <c r="H43" s="1">
+        <f>SUM(H38:H42)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <f>C47^2*PI()/4</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G47">
+        <f>(F47/D47)/(F$3/D$3)</f>
+        <v>1.2207446768156074</v>
+      </c>
+      <c r="H47" s="1">
+        <f>G47/$G$52</f>
+        <v>0.11444141689373298</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D48">
+        <f t="shared" ref="D48:D49" si="17">C48^2*PI()/4</f>
+        <v>7.0685834705770348E-2</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="G48">
+        <f>(F48/D48)/(F$3/D$3)</f>
+        <v>2.9065349447990654</v>
+      </c>
+      <c r="H48" s="1">
+        <f>G48/$G$52</f>
+        <v>0.27247956403269757</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="17"/>
+        <v>3.1415926535897934E-2</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="G49">
+        <f>(F49/D49)/(F$3/D$3)</f>
+        <v>6.5397036257978964</v>
+      </c>
+      <c r="H49" s="1">
+        <f>G49/$G$52</f>
+        <v>0.61307901907356954</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C50" s="2"/>
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C51" s="2"/>
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G52" s="3">
+        <f>SUM(G47:G51)</f>
+        <v>10.666983247412569</v>
+      </c>
+      <c r="H52" s="1">
+        <f>SUM(H47:H51)</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>